<commit_message>
Added import-file with hierarchy
</commit_message>
<xml_diff>
--- a/res_ssyk/data/ssyk-2012-koder.xlsx
+++ b/res_ssyk/data/ssyk-2012-koder.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\staff\Dropbox\projekt\Vertel_projekt\github-vertelab\odoo-base\res_ssyk\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2149794D-BB7B-47CE-9FBB-0D52EC16C760}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="8685" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hela strukturen" sheetId="4" r:id="rId1"/>
@@ -1898,7 +1892,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="00"/>
     <numFmt numFmtId="165" formatCode="000"/>
@@ -1989,7 +1983,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
@@ -2019,6 +2013,18 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2035,9 +2041,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2086,7 +2089,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2119,26 +2122,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2171,23 +2157,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2363,7 +2332,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F658"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7623,36 +7592,36 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B121" location="_ftn1" display="_ftn1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B218" location="_ftn2" display="_ftn2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B231" location="_ftn3" display="_ftn3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B264" location="_ftn4" display="_ftn4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B265" location="_ftn5" display="_ftn5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B279" location="_ftn6" display="_ftn6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B370" location="_ftn7" display="_ftn7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B406" location="_ftn8" display="_ftn8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B520" location="_ftn9" display="_ftn9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B625" location="_ftn10" display="_ftn10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B649" location="_ftnref1" display="_ftnref1" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B650" location="_ftnref2" display="_ftnref2" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B651" location="_ftnref3" display="_ftnref3" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B652" location="_ftnref4" display="_ftnref4" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B653" location="_ftnref5" display="_ftnref5" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B654" location="_ftnref6" display="_ftnref6" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B655" location="_ftnref7" display="_ftnref7" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B656" location="_ftnref8" display="_ftnref8" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B657" location="_ftnref9" display="_ftnref9" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B658" location="_ftnref10" display="_ftnref10" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B121" location="_ftn1" display="_ftn1"/>
+    <hyperlink ref="B218" location="_ftn2" display="_ftn2"/>
+    <hyperlink ref="B231" location="_ftn3" display="_ftn3"/>
+    <hyperlink ref="B264" location="_ftn4" display="_ftn4"/>
+    <hyperlink ref="B265" location="_ftn5" display="_ftn5"/>
+    <hyperlink ref="B279" location="_ftn6" display="_ftn6"/>
+    <hyperlink ref="B370" location="_ftn7" display="_ftn7"/>
+    <hyperlink ref="B406" location="_ftn8" display="_ftn8"/>
+    <hyperlink ref="B520" location="_ftn9" display="_ftn9"/>
+    <hyperlink ref="B625" location="_ftn10" display="_ftn10"/>
+    <hyperlink ref="B649" location="_ftnref1" display="_ftnref1"/>
+    <hyperlink ref="B650" location="_ftnref2" display="_ftnref2"/>
+    <hyperlink ref="B651" location="_ftnref3" display="_ftnref3"/>
+    <hyperlink ref="B652" location="_ftnref4" display="_ftnref4"/>
+    <hyperlink ref="B653" location="_ftnref5" display="_ftnref5"/>
+    <hyperlink ref="B654" location="_ftnref6" display="_ftnref6"/>
+    <hyperlink ref="B655" location="_ftnref7" display="_ftnref7"/>
+    <hyperlink ref="B656" location="_ftnref8" display="_ftnref8"/>
+    <hyperlink ref="B657" location="_ftnref9" display="_ftnref9"/>
+    <hyperlink ref="B658" location="_ftnref10" display="_ftnref10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -7814,7 +7783,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8226,7 +8195,7 @@
       <c r="C44" s="11"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="18">
+      <c r="A45" s="22">
         <v>1</v>
       </c>
       <c r="B45" s="12" t="s">
@@ -8235,7 +8204,7 @@
       <c r="C45" s="11"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="18">
+      <c r="A46" s="22">
         <v>2</v>
       </c>
       <c r="B46" s="12" t="s">
@@ -8244,7 +8213,7 @@
       <c r="C46" s="11"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="18">
+      <c r="A47" s="22">
         <v>3</v>
       </c>
       <c r="B47" s="12" t="s">
@@ -8307,10 +8276,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B163"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8319,7 +8290,7 @@
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>622</v>
       </c>
@@ -8327,1209 +8298,1949 @@
         <v>621</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>111</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>112</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>121</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>122</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>123</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>124</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>125</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>129</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>131</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>132</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>133</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>134</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>135</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>136</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>137</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>138</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>141</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>142</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>149</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>151</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>152</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>153</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>154</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>159</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>161</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
         <v>171</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
         <v>172</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
         <v>173</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
         <v>174</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
         <v>179</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="11">
         <v>211</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
         <v>212</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="11">
         <v>213</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="11">
         <v>214</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="11">
         <v>216</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="11">
         <v>217</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="11">
         <v>218</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="11">
         <v>221</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="11">
         <v>222</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="11">
         <v>223</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="11">
         <v>224</v>
       </c>
       <c r="B42" s="12" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="11">
         <v>225</v>
       </c>
       <c r="B43" s="12" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="11">
         <v>226</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="11">
         <v>227</v>
       </c>
       <c r="B45" s="12" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="11">
         <v>228</v>
       </c>
       <c r="B46" s="12" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="11">
         <v>231</v>
       </c>
       <c r="B47" s="12" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="11">
         <v>232</v>
       </c>
       <c r="B48" s="12" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="11">
         <v>233</v>
       </c>
       <c r="B49" s="12" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="11">
         <v>234</v>
       </c>
       <c r="B50" s="12" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="11">
         <v>235</v>
       </c>
       <c r="B51" s="12" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="11">
         <v>241</v>
       </c>
       <c r="B52" s="12" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="11">
         <v>242</v>
       </c>
       <c r="B53" s="12" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="11">
         <v>243</v>
       </c>
       <c r="B54" s="12" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="11">
         <v>251</v>
       </c>
       <c r="B55" s="12" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="11">
         <v>261</v>
       </c>
       <c r="B56" s="12" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="11">
         <v>262</v>
       </c>
       <c r="B57" s="12" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="11">
         <v>264</v>
       </c>
       <c r="B58" s="12" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="11">
         <v>265</v>
       </c>
       <c r="B59" s="12" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="11">
         <v>266</v>
       </c>
       <c r="B60" s="12" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="11">
         <v>267</v>
       </c>
       <c r="B61" s="12" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="11">
         <v>311</v>
       </c>
       <c r="B62" s="12" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="11">
         <v>312</v>
       </c>
       <c r="B63" s="12" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="11">
         <v>315</v>
       </c>
       <c r="B64" s="12" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="11">
         <v>321</v>
       </c>
       <c r="B65" s="12" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C65" s="11"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="11">
         <v>323</v>
       </c>
       <c r="B66" s="12" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="11">
         <v>324</v>
       </c>
       <c r="B67" s="12" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="11">
         <v>325</v>
       </c>
       <c r="B68" s="12" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C68" s="11"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="11">
         <v>331</v>
       </c>
       <c r="B69" s="12" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="11">
         <v>332</v>
       </c>
       <c r="B70" s="12" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="11">
         <v>333</v>
       </c>
       <c r="B71" s="12" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="11">
         <v>334</v>
       </c>
       <c r="B72" s="12" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C72" s="11"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="11">
         <v>335</v>
       </c>
       <c r="B73" s="12" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="11">
         <v>336</v>
       </c>
       <c r="B74" s="12" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C74" s="11"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="11"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="11">
         <v>341</v>
       </c>
       <c r="B75" s="12" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C75" s="11"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
+      <c r="G75" s="11"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="11">
         <v>342</v>
       </c>
       <c r="B76" s="12" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="11"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="11">
         <v>343</v>
       </c>
       <c r="B77" s="12" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="11">
         <v>344</v>
       </c>
       <c r="B78" s="12" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="11">
         <v>345</v>
       </c>
       <c r="B79" s="12" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C79" s="11"/>
+      <c r="D79" s="11"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="11">
         <v>351</v>
       </c>
       <c r="B80" s="12" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C80" s="11"/>
+      <c r="D80" s="11"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="11">
         <v>352</v>
       </c>
       <c r="B81" s="12" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C81" s="11"/>
+      <c r="D81" s="11"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="11"/>
+      <c r="G81" s="11"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="11">
         <v>411</v>
       </c>
       <c r="B82" s="12" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C82" s="11"/>
+      <c r="D82" s="20"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="11"/>
+      <c r="G82" s="11"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="11">
         <v>421</v>
       </c>
       <c r="B83" s="12" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C83" s="11"/>
+      <c r="D83" s="11"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="11"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="11">
         <v>422</v>
       </c>
       <c r="B84" s="12" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C84" s="11"/>
+      <c r="D84" s="11"/>
+      <c r="E84" s="11"/>
+      <c r="F84" s="11"/>
+      <c r="G84" s="11"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="11">
         <v>432</v>
       </c>
       <c r="B85" s="12" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
+      <c r="E85" s="11"/>
+      <c r="F85" s="11"/>
+      <c r="G85" s="11"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="11">
         <v>441</v>
       </c>
       <c r="B86" s="12" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C86" s="11"/>
+      <c r="D86" s="11"/>
+      <c r="E86" s="11"/>
+      <c r="F86" s="11"/>
+      <c r="G86" s="11"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="11">
         <v>442</v>
       </c>
       <c r="B87" s="12" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C87" s="11"/>
+      <c r="D87" s="11"/>
+      <c r="E87" s="11"/>
+      <c r="F87" s="11"/>
+      <c r="G87" s="11"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="11">
         <v>443</v>
       </c>
       <c r="B88" s="12" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C88" s="11"/>
+      <c r="D88" s="11"/>
+      <c r="E88" s="11"/>
+      <c r="F88" s="11"/>
+      <c r="G88" s="11"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="11">
         <v>511</v>
       </c>
       <c r="B89" s="12" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
+      <c r="E89" s="11"/>
+      <c r="F89" s="11"/>
+      <c r="G89" s="11"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="11">
         <v>512</v>
       </c>
       <c r="B90" s="12" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C90" s="11"/>
+      <c r="D90" s="11"/>
+      <c r="E90" s="11"/>
+      <c r="F90" s="11"/>
+      <c r="G90" s="11"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="11">
         <v>513</v>
       </c>
       <c r="B91" s="12" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C91" s="11"/>
+      <c r="D91" s="11"/>
+      <c r="E91" s="11"/>
+      <c r="F91" s="11"/>
+      <c r="G91" s="11"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="11">
         <v>514</v>
       </c>
       <c r="B92" s="12" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C92" s="11"/>
+      <c r="D92" s="11"/>
+      <c r="E92" s="11"/>
+      <c r="F92" s="11"/>
+      <c r="G92" s="11"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="11">
         <v>515</v>
       </c>
       <c r="B93" s="12" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C93" s="11"/>
+      <c r="D93" s="11"/>
+      <c r="E93" s="11"/>
+      <c r="F93" s="11"/>
+      <c r="G93" s="11"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="11">
         <v>516</v>
       </c>
       <c r="B94" s="12" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C94" s="11"/>
+      <c r="D94" s="11"/>
+      <c r="E94" s="11"/>
+      <c r="F94" s="11"/>
+      <c r="G94" s="11"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="11">
         <v>522</v>
       </c>
       <c r="B95" s="12" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C95" s="11"/>
+      <c r="D95" s="11"/>
+      <c r="E95" s="11"/>
+      <c r="F95" s="11"/>
+      <c r="G95" s="11"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="11">
         <v>523</v>
       </c>
       <c r="B96" s="12" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C96" s="11"/>
+      <c r="D96" s="11"/>
+      <c r="E96" s="11"/>
+      <c r="F96" s="11"/>
+      <c r="G96" s="11"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="11">
         <v>524</v>
       </c>
       <c r="B97" s="12" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C97" s="11"/>
+      <c r="D97" s="11"/>
+      <c r="E97" s="11"/>
+      <c r="F97" s="11"/>
+      <c r="G97" s="11"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="11">
         <v>531</v>
       </c>
       <c r="B98" s="12" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
+      <c r="E98" s="11"/>
+      <c r="F98" s="11"/>
+      <c r="G98" s="11"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="11">
         <v>532</v>
       </c>
       <c r="B99" s="12" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C99" s="11"/>
+      <c r="D99" s="11"/>
+      <c r="E99" s="17"/>
+      <c r="F99" s="11"/>
+      <c r="G99" s="11"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="11">
         <v>533</v>
       </c>
       <c r="B100" s="12" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C100" s="11"/>
+      <c r="D100" s="11"/>
+      <c r="E100" s="11"/>
+      <c r="F100" s="11"/>
+      <c r="G100" s="11"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="11">
         <v>534</v>
       </c>
       <c r="B101" s="12" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C101" s="11"/>
+      <c r="D101" s="11"/>
+      <c r="E101" s="11"/>
+      <c r="F101" s="11"/>
+      <c r="G101" s="11"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="11">
         <v>535</v>
       </c>
       <c r="B102" s="12" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C102" s="11"/>
+      <c r="D102" s="11"/>
+      <c r="E102" s="11"/>
+      <c r="F102" s="11"/>
+      <c r="G102" s="11"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="11">
         <v>541</v>
       </c>
       <c r="B103" s="12" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C103" s="11"/>
+      <c r="D103" s="11"/>
+      <c r="E103" s="11"/>
+      <c r="F103" s="11"/>
+      <c r="G103" s="11"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="11">
         <v>611</v>
       </c>
       <c r="B104" s="12" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C104" s="11"/>
+      <c r="D104" s="11"/>
+      <c r="E104" s="11"/>
+      <c r="F104" s="11"/>
+      <c r="G104" s="11"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="11">
         <v>612</v>
       </c>
       <c r="B105" s="12" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C105" s="11"/>
+      <c r="D105" s="11"/>
+      <c r="E105" s="11"/>
+      <c r="F105" s="11"/>
+      <c r="G105" s="11"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="11">
         <v>613</v>
       </c>
       <c r="B106" s="12" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C106" s="11"/>
+      <c r="D106" s="11"/>
+      <c r="E106" s="11"/>
+      <c r="F106" s="11"/>
+      <c r="G106" s="11"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="11">
         <v>621</v>
       </c>
       <c r="B107" s="12" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C107" s="11"/>
+      <c r="D107" s="11"/>
+      <c r="E107" s="11"/>
+      <c r="F107" s="11"/>
+      <c r="G107" s="11"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="11">
         <v>622</v>
       </c>
       <c r="B108" s="12" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C108" s="11"/>
+      <c r="D108" s="11"/>
+      <c r="E108" s="11"/>
+      <c r="F108" s="11"/>
+      <c r="G108" s="11"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="11">
         <v>711</v>
       </c>
       <c r="B109" s="12" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C109" s="11"/>
+      <c r="D109" s="11"/>
+      <c r="E109" s="11"/>
+      <c r="F109" s="11"/>
+      <c r="G109" s="11"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="11">
         <v>712</v>
       </c>
       <c r="B110" s="12" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C110" s="11"/>
+      <c r="D110" s="11"/>
+      <c r="E110" s="11"/>
+      <c r="F110" s="11"/>
+      <c r="G110" s="11"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="11">
         <v>713</v>
       </c>
       <c r="B111" s="12" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C111" s="11"/>
+      <c r="D111" s="11"/>
+      <c r="E111" s="11"/>
+      <c r="F111" s="11"/>
+      <c r="G111" s="11"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="11">
         <v>721</v>
       </c>
       <c r="B112" s="12" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
+      <c r="E112" s="11"/>
+      <c r="F112" s="11"/>
+      <c r="G112" s="11"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="11">
         <v>722</v>
       </c>
       <c r="B113" s="12" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
+      <c r="E113" s="11"/>
+      <c r="F113" s="11"/>
+      <c r="G113" s="11"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="11">
         <v>723</v>
       </c>
       <c r="B114" s="12" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C114" s="11"/>
+      <c r="D114" s="11"/>
+      <c r="E114" s="11"/>
+      <c r="F114" s="11"/>
+      <c r="G114" s="11"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="11">
         <v>731</v>
       </c>
       <c r="B115" s="12" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C115" s="11"/>
+      <c r="D115" s="11"/>
+      <c r="E115" s="11"/>
+      <c r="F115" s="11"/>
+      <c r="G115" s="11"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="11">
         <v>732</v>
       </c>
       <c r="B116" s="12" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C116" s="11"/>
+      <c r="D116" s="11"/>
+      <c r="E116" s="17"/>
+      <c r="F116" s="11"/>
+      <c r="G116" s="11"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="11">
         <v>741</v>
       </c>
       <c r="B117" s="12" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C117" s="11"/>
+      <c r="D117" s="11"/>
+      <c r="E117" s="17"/>
+      <c r="F117" s="11"/>
+      <c r="G117" s="11"/>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="11">
         <v>742</v>
       </c>
       <c r="B118" s="12" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C118" s="11"/>
+      <c r="D118" s="11"/>
+      <c r="E118" s="11"/>
+      <c r="F118" s="11"/>
+      <c r="G118" s="11"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="11">
         <v>752</v>
       </c>
       <c r="B119" s="12" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C119" s="11"/>
+      <c r="D119" s="11"/>
+      <c r="E119" s="11"/>
+      <c r="F119" s="11"/>
+      <c r="G119" s="11"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="11">
         <v>753</v>
       </c>
       <c r="B120" s="12" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C120" s="11"/>
+      <c r="D120" s="11"/>
+      <c r="E120" s="11"/>
+      <c r="F120" s="11"/>
+      <c r="G120" s="11"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="11">
         <v>761</v>
       </c>
       <c r="B121" s="12" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C121" s="11"/>
+      <c r="D121" s="11"/>
+      <c r="E121" s="11"/>
+      <c r="F121" s="11"/>
+      <c r="G121" s="11"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" s="11">
         <v>811</v>
       </c>
       <c r="B122" s="12" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C122" s="11"/>
+      <c r="D122" s="11"/>
+      <c r="E122" s="11"/>
+      <c r="F122" s="11"/>
+      <c r="G122" s="11"/>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" s="11">
         <v>812</v>
       </c>
       <c r="B123" s="12" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C123" s="11"/>
+      <c r="D123" s="11"/>
+      <c r="E123" s="11"/>
+      <c r="F123" s="11"/>
+      <c r="G123" s="11"/>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="11">
         <v>813</v>
       </c>
       <c r="B124" s="12" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C124" s="11"/>
+      <c r="D124" s="11"/>
+      <c r="E124" s="11"/>
+      <c r="F124" s="11"/>
+      <c r="G124" s="11"/>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="11">
         <v>814</v>
       </c>
       <c r="B125" s="12" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C125" s="11"/>
+      <c r="D125" s="11"/>
+      <c r="E125" s="11"/>
+      <c r="F125" s="11"/>
+      <c r="G125" s="11"/>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" s="11">
         <v>815</v>
       </c>
       <c r="B126" s="12" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C126" s="11"/>
+      <c r="D126" s="11"/>
+      <c r="E126" s="11"/>
+      <c r="F126" s="11"/>
+      <c r="G126" s="11"/>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" s="11">
         <v>816</v>
       </c>
       <c r="B127" s="12" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C127" s="11"/>
+      <c r="D127" s="11"/>
+      <c r="E127" s="17"/>
+      <c r="F127" s="11"/>
+      <c r="G127" s="11"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="11">
         <v>817</v>
       </c>
       <c r="B128" s="12" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C128" s="11"/>
+      <c r="D128" s="11"/>
+      <c r="E128" s="11"/>
+      <c r="F128" s="11"/>
+      <c r="G128" s="11"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" s="11">
         <v>818</v>
       </c>
       <c r="B129" s="12" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C129" s="11"/>
+      <c r="D129" s="11"/>
+      <c r="E129" s="11"/>
+      <c r="F129" s="11"/>
+      <c r="G129" s="11"/>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="11">
         <v>819</v>
       </c>
       <c r="B130" s="12" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C130" s="11"/>
+      <c r="D130" s="11"/>
+      <c r="E130" s="11"/>
+      <c r="F130" s="11"/>
+      <c r="G130" s="11"/>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" s="11">
         <v>821</v>
       </c>
       <c r="B131" s="12" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C131" s="11"/>
+      <c r="D131" s="11"/>
+      <c r="E131" s="17"/>
+      <c r="F131" s="11"/>
+      <c r="G131" s="11"/>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" s="11">
         <v>831</v>
       </c>
       <c r="B132" s="12" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C132" s="11"/>
+      <c r="D132" s="11"/>
+      <c r="E132" s="11"/>
+      <c r="F132" s="11"/>
+      <c r="G132" s="11"/>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="11">
         <v>832</v>
       </c>
       <c r="B133" s="12" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C133" s="11"/>
+      <c r="D133" s="11"/>
+      <c r="E133" s="11"/>
+      <c r="F133" s="11"/>
+      <c r="G133" s="11"/>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" s="11">
         <v>833</v>
       </c>
       <c r="B134" s="12" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C134" s="11"/>
+      <c r="D134" s="11"/>
+      <c r="E134" s="11"/>
+      <c r="F134" s="11"/>
+      <c r="G134" s="11"/>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" s="11">
         <v>834</v>
       </c>
       <c r="B135" s="12" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C135" s="11"/>
+      <c r="D135" s="11"/>
+      <c r="E135" s="11"/>
+      <c r="F135" s="11"/>
+      <c r="G135" s="11"/>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="11">
         <v>835</v>
       </c>
       <c r="B136" s="12" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C136" s="11"/>
+      <c r="D136" s="11"/>
+      <c r="E136" s="11"/>
+      <c r="F136" s="11"/>
+      <c r="G136" s="11"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="11">
         <v>911</v>
       </c>
       <c r="B137" s="12" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C137" s="11"/>
+      <c r="D137" s="11"/>
+      <c r="E137" s="11"/>
+      <c r="F137" s="11"/>
+      <c r="G137" s="11"/>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="11">
         <v>912</v>
       </c>
       <c r="B138" s="12" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C138" s="11"/>
+      <c r="D138" s="11"/>
+      <c r="E138" s="17"/>
+      <c r="F138" s="11"/>
+      <c r="G138" s="11"/>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" s="11">
         <v>921</v>
       </c>
       <c r="B139" s="12" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C139" s="11"/>
+      <c r="D139" s="11"/>
+      <c r="E139" s="11"/>
+      <c r="F139" s="11"/>
+      <c r="G139" s="11"/>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" s="11">
         <v>931</v>
       </c>
       <c r="B140" s="12" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C140" s="11"/>
+      <c r="D140" s="11"/>
+      <c r="E140" s="11"/>
+      <c r="F140" s="11"/>
+      <c r="G140" s="11"/>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" s="11">
         <v>932</v>
       </c>
       <c r="B141" s="12" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C141" s="11"/>
+      <c r="D141" s="11"/>
+      <c r="E141" s="11"/>
+      <c r="F141" s="11"/>
+      <c r="G141" s="11"/>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" s="11">
         <v>933</v>
       </c>
       <c r="B142" s="12" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C142" s="11"/>
+      <c r="D142" s="11"/>
+      <c r="E142" s="11"/>
+      <c r="F142" s="11"/>
+      <c r="G142" s="11"/>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" s="11">
         <v>941</v>
       </c>
       <c r="B143" s="12" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C143" s="11"/>
+      <c r="D143" s="11"/>
+      <c r="E143" s="11"/>
+      <c r="F143" s="11"/>
+      <c r="G143" s="11"/>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" s="11">
         <v>952</v>
       </c>
       <c r="B144" s="12" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C144" s="11"/>
+      <c r="D144" s="11"/>
+      <c r="E144" s="11"/>
+      <c r="F144" s="11"/>
+      <c r="G144" s="11"/>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" s="11">
         <v>961</v>
       </c>
       <c r="B145" s="12" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C145" s="11"/>
+      <c r="D145" s="11"/>
+      <c r="E145" s="11"/>
+      <c r="F145" s="11"/>
+      <c r="G145" s="11"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" s="11">
         <v>962</v>
       </c>
       <c r="B146" s="12" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" s="17">
+      <c r="C146" s="11"/>
+      <c r="D146" s="11"/>
+      <c r="E146" s="11"/>
+      <c r="F146" s="11"/>
+      <c r="G146" s="11"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A147" s="21">
         <v>11</v>
       </c>
       <c r="B147" s="12" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" s="17">
+      <c r="C147" s="11"/>
+      <c r="D147" s="11"/>
+      <c r="E147" s="11"/>
+      <c r="F147" s="11"/>
+      <c r="G147" s="11"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A148" s="21">
         <v>21</v>
       </c>
       <c r="B148" s="12" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" s="17">
+      <c r="C148" s="11"/>
+      <c r="D148" s="11"/>
+      <c r="E148" s="11"/>
+      <c r="F148" s="11"/>
+      <c r="G148" s="11"/>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A149" s="21">
         <v>31</v>
       </c>
       <c r="B149" s="12" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C149" s="11"/>
+      <c r="D149" s="11"/>
+      <c r="E149" s="11"/>
+      <c r="F149" s="11"/>
+      <c r="G149" s="11"/>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B154" s="9"/>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B155" s="9"/>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B156" s="9"/>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B157" s="9"/>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B158" s="9"/>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B159" s="9"/>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B160" s="9"/>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.2">
@@ -9547,7 +10258,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B444"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>